<commit_message>
Reworked Task classes and added some more general tasks
</commit_message>
<xml_diff>
--- a/SettlerAIMutexes.xlsx
+++ b/SettlerAIMutexes.xlsx
@@ -399,7 +399,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,7 +502,7 @@
       </c>
       <c r="C4">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -511,7 +511,7 @@
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -622,13 +622,13 @@
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -652,19 +652,19 @@
       </c>
       <c r="C9">
         <f t="shared" si="0"/>
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9">
         <v>1</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9">
         <v>0</v>
@@ -742,7 +742,7 @@
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -751,7 +751,7 @@
         <v>0</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H12">
         <v>0</v>

</xml_diff>